<commit_message>
(Result files): Adding missing result files after final analysis for master thesis
</commit_message>
<xml_diff>
--- a/code/results/Participants/Analysis/Jamovi_analysis/Dobot_gest_V1.0_work_edition.xlsx
+++ b/code/results/Participants/Analysis/Jamovi_analysis/Dobot_gest_V1.0_work_edition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -615,7 +615,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY\ H:MM:SS"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -645,25 +645,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="13"/>
@@ -685,6 +672,7 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -729,7 +717,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -746,30 +734,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -834,7 +818,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -847,11 +831,27 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Pointing action survey responses</a:t>
@@ -860,12 +860,6 @@
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -897,23 +891,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -976,23 +959,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1033,11 +1005,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="25351336"/>
-        <c:axId val="79722162"/>
+        <c:axId val="21114140"/>
+        <c:axId val="99670430"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25351336"/>
+        <c:axId val="21114140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,23 +1028,30 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79722162"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="99670430"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79722162"/>
+        <c:axId val="99670430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1096,11 +1075,27 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>sum of mentions </a:t>
@@ -1112,19 +1107,13 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0426875"/>
-              <c:y val="0.512222222222222"/>
+              <c:x val="0.0426585412302419"/>
+              <c:y val="0.512056895210579"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1137,17 +1126,25 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25351336"/>
+        <c:crossAx val="21114140"/>
         <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1167,17 +1164,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1193,7 +1179,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1206,11 +1192,27 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Planning action survey responses</a:t>
@@ -1219,12 +1221,6 @@
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1256,23 +1252,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1341,23 +1326,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1404,11 +1378,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="22581503"/>
-        <c:axId val="49254787"/>
+        <c:axId val="93107119"/>
+        <c:axId val="51299884"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22581503"/>
+        <c:axId val="93107119"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,23 +1401,30 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49254787"/>
+        <c:crossAx val="51299884"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49254787"/>
+        <c:axId val="51299884"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1467,11 +1448,27 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>sum of mentions </a:t>
@@ -1483,19 +1480,13 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0205625"/>
-              <c:y val="0.529888888888889"/>
+              <c:x val="0.0205722243321939"/>
+              <c:y val="0.52972552505834"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1508,17 +1499,25 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22581503"/>
+        <c:crossAx val="93107119"/>
         <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1538,17 +1537,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1564,7 +1552,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1577,11 +1565,27 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Grasping, cancel and idle action survey responses</a:t>
@@ -1590,12 +1594,6 @@
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1627,23 +1625,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1718,23 +1705,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1809,23 +1785,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1878,11 +1843,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="23071740"/>
-        <c:axId val="79573176"/>
+        <c:axId val="66564945"/>
+        <c:axId val="81388490"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23071740"/>
+        <c:axId val="66564945"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,23 +1866,30 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79573176"/>
+        <c:crossAx val="81388490"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79573176"/>
+        <c:axId val="81388490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1941,11 +1913,27 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>sum of mentions</a:t>
@@ -1957,19 +1945,13 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.06625"/>
-              <c:y val="0.524888888888889"/>
+              <c:x val="0.0662197204477895"/>
+              <c:y val="0.524836092899211"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1982,17 +1964,25 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23071740"/>
+        <c:crossAx val="66564945"/>
         <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2012,17 +2002,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2049,9 +2028,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2060,7 +2039,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2019960" y="7048440"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5670720" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2084,9 +2063,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>729360</xdr:colOff>
+      <xdr:colOff>729000</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2094,8 +2073,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1817280" y="7743960"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="1785600" y="7743960"/>
+        <a:ext cx="5686920" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2119,9 +2098,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>428760</xdr:colOff>
+      <xdr:colOff>428400</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2129,8 +2108,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="835560" y="7641720"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="822960" y="7641720"/>
+        <a:ext cx="5691600" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2150,16 +2129,16 @@
   </sheetPr>
   <dimension ref="A1:BP13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="1" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="75" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="74" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="75" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4666,7 +4645,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4679,28 +4658,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="3" t="str">
         <f aca="false">'Form Responses 1'!BM1</f>
-        <v>2-4: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-4: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="D1" s="4" t="str">
         <f aca="false">'Form Responses 1'!BN1</f>
-        <v>2-5: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-5: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -4916,7 +4895,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -4928,7 +4907,7 @@
       <c r="C20" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E20" s="5"/>
@@ -4983,11 +4962,11 @@
       <c r="B23" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C23" s="6" t="n">
+      <c r="C23" s="5" t="n">
         <f aca="false">COUNTIF(C2:C13,A23)</f>
         <v>1</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D23" s="5" t="n">
         <f aca="false">COUNTIF(D2:D13,A23)</f>
         <v>0</v>
       </c>
@@ -4996,143 +4975,10 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5146,29 +4992,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="3" t="str">
         <f aca="false">'Form Responses 1'!BK1</f>
-        <v>2-2: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-2: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="D1" s="4" t="str">
         <f aca="false">'Form Responses 1'!BP1</f>
-        <v>2-7: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-7: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -5373,7 +5219,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -5384,7 +5230,7 @@
       <c r="C21" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E21" s="3"/>
@@ -5436,11 +5282,11 @@
       <c r="B24" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="6" t="n">
+      <c r="C24" s="5" t="n">
         <f aca="false">COUNTIF(C2:C14,A24)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D24" s="5" t="n">
         <f aca="false">COUNTIF(D2:D14,A24)</f>
         <v>2</v>
       </c>
@@ -5467,94 +5313,10 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5568,20 +5330,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5600,15 +5362,15 @@
     <row r="2" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="4" t="str">
         <f aca="false">'Form Responses 1'!BJ1</f>
-        <v>2-1: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-1: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="D2" s="4" t="str">
         <f aca="false">'Form Responses 1'!BL1</f>
-        <v>2-3: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-3: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="E2" s="4" t="str">
         <f aca="false">'Form Responses 1'!BO1</f>
-        <v>2-6: Which of the sentences explains the gesture you just saw best? </v>
+        <v>2-6: Which of the sentences explains the gesture you just saw best?</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5855,7 +5617,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -5866,7 +5628,7 @@
       <c r="C23" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>191</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -5942,7 +5704,7 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -5964,7 +5726,7 @@
       <c r="G27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -5985,67 +5747,10 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>